<commit_message>
Add no mitigation WAM/WEM scenarios
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_IND_Shares.xlsx
+++ b/SuppXLS/Scen_B_IND_Shares.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbsul\Documents\GitHub\times-ireland-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5965E5-6FC1-460E-98A1-49AFE323707F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A45167F-001C-4415-BA4B-2202657041E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="19200" windowHeight="11170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IND" sheetId="2" r:id="rId1"/>
@@ -314,10 +314,10 @@
     <t>I*CEM*RWS*,-I*DRR*RWS*</t>
   </si>
   <si>
-    <t>I*CEM*NWS*-I*DRR*RWS*</t>
-  </si>
-  <si>
     <t>I*WS*,-I*CEM*WS*,-I*LIM*WS*</t>
+  </si>
+  <si>
+    <t>I*CEM*NWS*,-I*DRR*RWS*</t>
   </si>
 </sst>
 </file>
@@ -2792,7 +2792,7 @@
   <dimension ref="C3:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2877,7 +2877,7 @@
         <v>0.2</v>
       </c>
       <c r="J6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K6" t="s">
         <v>57</v>
@@ -2901,7 +2901,7 @@
         <v>0.01</v>
       </c>
       <c r="J7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K7" t="s">
         <v>57</v>

</xml_diff>